<commit_message>
fixes for exercise 2
fixed repo and copy and pasted Nasir's work back in :)
</commit_message>
<xml_diff>
--- a/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
+++ b/starter-analysis-exercise/data/raw-data/exampledata2.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10112"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269E5E2B-6FD3-A94D-8B8E-21CE2A84DE9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD858DD3-5FA6-AA45-B898-5A0A876019D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -430,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="187" zoomScaleNormal="187" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView zoomScale="187" zoomScaleNormal="187" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -697,7 +697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4A2C8F0-62B4-4D60-B490-D490A3E0B40F}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>

</xml_diff>